<commit_message>
journal de travail valentin
</commit_message>
<xml_diff>
--- a/documentation/306_Journal_travail_ArcardiaBox_GREMAUD_VALENTIN.xlsx
+++ b/documentation/306_Journal_travail_ArcardiaBox_GREMAUD_VALENTIN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/valentin_gremaud_studentfr_ch/Documents/Documents/INFO/3ème année/306/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{542619C4-930E-734D-95CD-9EBCC3E78C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5E30509-1304-8842-902C-057A5AA26084}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{AD3704F4-E514-C94B-BB1C-897372BB263A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15E5DC2A-9D9B-9B43-84AD-956FBBAD9100}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="8" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>Gremaud Valentin</t>
   </si>
@@ -119,6 +119,48 @@
   </si>
   <si>
     <t>J'ai bien bossé aujourd'hui, je crois avoir bien rempli mon travail de product owner en ayant défini l'objectif de notre sprint et m'étant assuré que chacun ait du travail. J'ai peu codé ou travaillé concrètement sur le projet hors mis que j'ai aidé diogo dans la config.</t>
+  </si>
+  <si>
+    <t>Documentation de la conception</t>
+  </si>
+  <si>
+    <t>Configuration de la Raspberry</t>
+  </si>
+  <si>
+    <t>Installation du serveur web sur la raspberry</t>
+  </si>
+  <si>
+    <t>Déploiement sur la raspberry du PACMAN</t>
+  </si>
+  <si>
+    <t>Test du jeu déployé (Bug de fluidité)</t>
+  </si>
+  <si>
+    <t>Changement d'OS sur la raspberry pour optimiser la fluidité</t>
+  </si>
+  <si>
+    <t>Lecture du cahier des charges</t>
+  </si>
+  <si>
+    <t>Création d'un business case</t>
+  </si>
+  <si>
+    <t>Rencontre avec le client (kick-off)</t>
+  </si>
+  <si>
+    <t>Préparation de la rencontre avec client</t>
+  </si>
+  <si>
+    <t>Documentation initiale</t>
+  </si>
+  <si>
+    <t>Aide à Axelle pour le planning</t>
+  </si>
+  <si>
+    <t>Users stories et product backlog</t>
+  </si>
+  <si>
+    <t>C'était la semaine de lancement du projet donc je n'ai pas forcément fait énormément de travail mais j'ai surtout réfléchi comment mener à bien le projet de la meilleure manière.</t>
   </si>
 </sst>
 </file>
@@ -576,10 +618,22 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -642,18 +696,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1162,10 +1204,10 @@
   <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E23" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E35" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="A33" sqref="A33:D33"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A19:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1182,20 +1224,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
       <c r="H2" s="15"/>
       <c r="I2" s="1" t="s">
         <v>1</v>
@@ -1208,13 +1250,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="41"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1224,9 +1266,9 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="43"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1236,18 +1278,26 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="47">
+      <c r="A6" s="50">
         <v>45992</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="6"/>
+      <c r="B6" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="48"/>
+      <c r="D6" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="18"/>
-      <c r="B7" s="21"/>
+      <c r="B7" s="21" t="s">
+        <v>26</v>
+      </c>
       <c r="C7" s="22"/>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="18"/>
@@ -1263,7 +1313,7 @@
       </c>
       <c r="D9" s="8">
         <f>SUM(D6:D8)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1276,15 +1326,23 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="18"/>
-      <c r="B11" s="21"/>
+      <c r="B11" s="21" t="s">
+        <v>30</v>
+      </c>
       <c r="C11" s="22"/>
-      <c r="D11" s="7"/>
+      <c r="D11" s="7">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="18"/>
-      <c r="B12" s="21"/>
+      <c r="B12" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="C12" s="22"/>
-      <c r="D12" s="7"/>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="18"/>
@@ -1294,28 +1352,40 @@
       </c>
       <c r="D13" s="8">
         <f>SUM(D10:D12)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="17">
         <v>45993</v>
       </c>
-      <c r="B14" s="19"/>
+      <c r="B14" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="C14" s="20"/>
-      <c r="D14" s="6"/>
+      <c r="D14" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="18"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="7"/>
+      <c r="B15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="7">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="18"/>
-      <c r="B16" s="21"/>
+      <c r="B16" s="21" t="s">
+        <v>29</v>
+      </c>
       <c r="C16" s="22"/>
-      <c r="D16" s="7"/>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="18"/>
@@ -1325,7 +1395,7 @@
       </c>
       <c r="D17" s="8">
         <f>SUM(D14:D16)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
@@ -1338,11 +1408,13 @@
       </c>
       <c r="D18" s="11">
         <f>SUM(D9,D13,D17)</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="28"/>
+      <c r="A19" s="31" t="s">
+        <v>32</v>
+      </c>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
       <c r="D19" s="30"/>
@@ -1351,22 +1423,22 @@
       <c r="A20" s="18">
         <v>45999</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="33"/>
+      <c r="C20" s="36"/>
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="18"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="38"/>
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="18"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="37"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
@@ -1384,22 +1456,22 @@
       <c r="A24" s="17">
         <v>45999</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="33"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="18"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="38"/>
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="18"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="40"/>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
@@ -1427,10 +1499,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="18"/>
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="49"/>
+      <c r="C29" s="34"/>
       <c r="D29" s="7">
         <v>1</v>
       </c>
@@ -1470,7 +1542,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="50" t="s">
+      <c r="A33" s="31" t="s">
         <v>18</v>
       </c>
       <c r="B33" s="29"/>
@@ -1478,24 +1550,36 @@
       <c r="D33" s="30"/>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="31">
+      <c r="A34" s="32">
         <v>46006</v>
       </c>
-      <c r="B34" s="19"/>
+      <c r="B34" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="C34" s="20"/>
-      <c r="D34" s="7"/>
+      <c r="D34" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="18"/>
-      <c r="B35" s="21"/>
+      <c r="B35" s="21" t="s">
+        <v>20</v>
+      </c>
       <c r="C35" s="22"/>
-      <c r="D35" s="7"/>
+      <c r="D35" s="7">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="18"/>
-      <c r="B36" s="21"/>
+      <c r="B36" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="C36" s="22"/>
-      <c r="D36" s="7"/>
+      <c r="D36" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="18"/>
@@ -1505,28 +1589,40 @@
       </c>
       <c r="D37" s="8">
         <f>SUM(D34:D36)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="17">
         <v>46006</v>
       </c>
-      <c r="B38" s="19"/>
+      <c r="B38" s="19" t="s">
+        <v>22</v>
+      </c>
       <c r="C38" s="20"/>
-      <c r="D38" s="6"/>
+      <c r="D38" s="6">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="18"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="7"/>
+      <c r="B39" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="15"/>
+      <c r="D39" s="7">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="18"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="7"/>
+      <c r="B40" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="16"/>
+      <c r="D40" s="7">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="18"/>
@@ -1536,7 +1632,7 @@
       </c>
       <c r="D41" s="8">
         <f>SUM(D38:D40)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1580,7 +1676,7 @@
       </c>
       <c r="D46" s="11">
         <f>SUM(D37,D41,D45)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.15">
@@ -1813,11 +1909,11 @@
       </c>
       <c r="D76" s="9">
         <f>D18+D32+D46+D60+D74</f>
-        <v>3.5</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="69">
+  <mergeCells count="66">
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
@@ -1842,7 +1938,6 @@
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B20:C22"/>
     <mergeCell ref="A24:A27"/>
@@ -1856,8 +1951,6 @@
     <mergeCell ref="A34:A37"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="A47:D47"/>
     <mergeCell ref="A48:A51"/>
@@ -1951,81 +2044,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <AppVersion xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Invited_Students xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Owner xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Teams_Channel_Section_Location xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <TeamsChannelId xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Invited_Teachers xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <FolderType xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <CultureName xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Student_Groups xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Self_Registration_Enabled xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Teachers xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Students xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Templates xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <LMS_Mappings xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <NotebookType xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Distribution_Groups xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Math_Settings xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <TaxCatchAll xmlns="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5" xsi:nil="true"/>
-    <SharedWithUsers xmlns="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Groupe xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Langue xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">FD = français voie bili</Langue>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100280ED870E36F6F4C976CEAC6988F82A5" ma:contentTypeVersion="37" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3169f06de23f2334ced166a676265d3f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xmlns:ns3="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eab9665bb0af9cfdaba242b84d69e760" ns2:_="" ns3:_="">
     <xsd:import namespace="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea"/>
@@ -2462,32 +2480,82 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34A0F71E-9B9F-4628-8A94-D320BA80A1D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A574440-4762-4322-B305-C51AEF435DC1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5"/>
-    <ds:schemaRef ds:uri="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <AppVersion xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Invited_Students xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Owner xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Teams_Channel_Section_Location xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <TeamsChannelId xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Invited_Teachers xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <FolderType xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <CultureName xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Student_Groups xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Self_Registration_Enabled xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Teachers xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Students xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Templates xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <LMS_Mappings xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <NotebookType xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Distribution_Groups xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Math_Settings xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <TaxCatchAll xmlns="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5" xsi:nil="true"/>
+    <SharedWithUsers xmlns="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Groupe xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Langue xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">FD = français voie bili</Langue>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA445AE9-3816-4E66-9DE6-AF42B0662460}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2504,4 +2572,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34A0F71E-9B9F-4628-8A94-D320BA80A1D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A574440-4762-4322-B305-C51AEF435DC1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>